<commit_message>
updated file including 2pom
</commit_message>
<xml_diff>
--- a/VTiger/testData/testScriptData.xlsx
+++ b/VTiger/testData/testScriptData.xlsx
@@ -1,24 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SR Studio\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF5A6A7E-7FC7-4506-9E09-C52E3151AE92}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13935" windowHeight="3630" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="org" sheetId="1" r:id="rId1"/>
     <sheet name="contact" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="124519"/>
+  <oleSize ref="B1:E5"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -26,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="20">
   <si>
     <t>testID</t>
   </si>
@@ -71,19 +66,40 @@
   </si>
   <si>
     <t>deepak</t>
+  </si>
+  <si>
+    <t>test_03</t>
+  </si>
+  <si>
+    <t>deletingOrganization</t>
+  </si>
+  <si>
+    <t>No Organization Found !</t>
+  </si>
+  <si>
+    <t>deletingContWithOrg</t>
+  </si>
+  <si>
+    <t>No Contact Found !</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -127,10 +143,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -191,7 +208,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -226,7 +243,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -403,27 +420,27 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="25.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -443,7 +460,7 @@
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -463,7 +480,7 @@
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -478,7 +495,7 @@
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8">
       <c r="A5" s="2" t="s">
         <v>10</v>
       </c>
@@ -493,26 +510,41 @@
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
     </row>
+    <row r="7" spans="1:8">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB901F64-B97D-4099-B7B0-E50AA34C6726}">
-  <dimension ref="A1:G2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="25.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -533,7 +565,7 @@
       </c>
       <c r="G1" s="1"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -554,7 +586,28 @@
       </c>
       <c r="G2" s="2"/>
     </row>
+    <row r="3" spans="1:7">
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>